<commit_message>
Commit for Subject exam wizard
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CategorySubjectMappingData" sheetId="1" r:id="rId1"/>
     <sheet name="CategorySubMapping_GridView" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="ExamSubjectWizardData" sheetId="4" r:id="rId3"/>
+    <sheet name="MarksEntry_ExamSubjectWizard" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:M19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Academic Year</t>
   </si>
@@ -47,6 +47,30 @@
   </si>
   <si>
     <t>2018-2019</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>UKG - EXAM</t>
+  </si>
+  <si>
+    <t>Pre Nursery</t>
+  </si>
+  <si>
+    <t>Max Marks</t>
+  </si>
+  <si>
+    <t>Min Marks</t>
+  </si>
+  <si>
+    <t>Max Entry Marks</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -455,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,12 +525,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit for exam login privilege
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
@@ -4,20 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="CategorySubjectMappingData" sheetId="1" r:id="rId1"/>
     <sheet name="CategorySubMapping_GridView" sheetId="2" r:id="rId2"/>
-    <sheet name="ExamSubjectWizardData" sheetId="4" r:id="rId3"/>
-    <sheet name="MarksEntry_ExamSubjectWizard" sheetId="5" r:id="rId4"/>
+    <sheet name="ExamSubjectWizard_GradeDisplay" sheetId="4" r:id="rId3"/>
+    <sheet name="ExamSubjectWizard_MarksDisplay" sheetId="11" r:id="rId4"/>
+    <sheet name="ExamSubjectWizard_SubExamSubj" sheetId="12" r:id="rId5"/>
+    <sheet name="MarksEntry_ExamSubjectWizard" sheetId="5" r:id="rId6"/>
+    <sheet name="SubExamWindow_MarksEntry_Sub1" sheetId="7" r:id="rId7"/>
+    <sheet name="SubExamWindow_MarksEntry_Sub2" sheetId="8" r:id="rId8"/>
+    <sheet name="SubSubjectWin_MarksEntry_Sub1" sheetId="9" r:id="rId9"/>
+    <sheet name="FilterRecords_ExamSubjectWizard" sheetId="10" r:id="rId10"/>
+    <sheet name="ExamLoginPrivilege_ClassT" sheetId="13" r:id="rId11"/>
+    <sheet name="ExamLoginPrivilege_SubjectT" sheetId="14" r:id="rId12"/>
+    <sheet name="ExamLoginPrivilege_GridView" sheetId="15" r:id="rId13"/>
+    <sheet name="ExamStudentMappingData" sheetId="16" r:id="rId14"/>
+    <sheet name="Search_StudentMapping" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="51">
   <si>
     <t>Academic Year</t>
   </si>
@@ -71,6 +82,105 @@
   </si>
   <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>SubExam MaxMarks</t>
+  </si>
+  <si>
+    <t>AubExam MinMarks</t>
+  </si>
+  <si>
+    <t>subExam Grade</t>
+  </si>
+  <si>
+    <t>SubExam ExemptedPercentage</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Exam Name</t>
+  </si>
+  <si>
+    <t>Grade Name</t>
+  </si>
+  <si>
+    <t>FINAL EXAM</t>
+  </si>
+  <si>
+    <t>New Pre Nursery</t>
+  </si>
+  <si>
+    <t>New Pre Nursery-1</t>
+  </si>
+  <si>
+    <t>New Pre Nursery-2</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>SubSubject</t>
+  </si>
+  <si>
+    <t>MRS ANITHA JAMES</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>English Grammer</t>
+  </si>
+  <si>
+    <t>MRS JAMUNA PAVAN</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AcademicYear</t>
+  </si>
+  <si>
+    <t>ExamCategory</t>
+  </si>
+  <si>
+    <t>Class_SM</t>
+  </si>
+  <si>
+    <t>Section_SM</t>
+  </si>
+  <si>
+    <t>UKG</t>
+  </si>
+  <si>
+    <t>StudentName</t>
+  </si>
+  <si>
+    <t>LKG</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BHARATH NANDHAN K</t>
   </si>
 </sst>
 </file>
@@ -121,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,6 +245,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,6 +590,355 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
@@ -528,13 +992,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -558,8 +1023,8 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -575,7 +1040,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -617,4 +1178,168 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit for latest commit
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="CategorySubjectMappingData" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="ExamLoginPrivilege_GridView" sheetId="15" r:id="rId13"/>
     <sheet name="ExamStudentMappingData" sheetId="16" r:id="rId14"/>
     <sheet name="Search_StudentMapping" sheetId="18" r:id="rId15"/>
+    <sheet name="Exam_SubjectWizardGradeDisp" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
   <si>
     <t>Academic Year</t>
   </si>
@@ -120,9 +121,6 @@
     <t>New Pre Nursery-1</t>
   </si>
   <si>
-    <t>New Pre Nursery-2</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -135,9 +133,6 @@
     <t>SubSubject</t>
   </si>
   <si>
-    <t>MRS ANITHA JAMES</t>
-  </si>
-  <si>
     <t>ENGLISH</t>
   </si>
   <si>
@@ -182,12 +177,27 @@
   <si>
     <t>BHARATH NANDHAN K</t>
   </si>
+  <si>
+    <t>UKG - Exam</t>
+  </si>
+  <si>
+    <t>AnithaJames : 2007029</t>
+  </si>
+  <si>
+    <t>MRS ANITHA JAMES : 2007029</t>
+  </si>
+  <si>
+    <t>Priya : 123456</t>
+  </si>
+  <si>
+    <t>Priya Baskar : 123456</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +220,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,12 +266,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -334,6 +359,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -368,6 +394,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,20 +570,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -570,7 +597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -591,21 +618,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -622,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -646,56 +673,57 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
@@ -707,57 +735,58 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>38</v>
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -765,52 +794,53 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -823,14 +853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -838,27 +868,27 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -869,16 +899,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -889,14 +919,100 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,57 +1020,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -968,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -988,21 +1069,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1037,21 +1118,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1085,21 +1166,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -1133,21 +1214,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1181,21 +1262,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1212,7 +1293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1235,21 +1316,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1290,14 +1371,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1305,7 +1386,7 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1322,7 +1403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Changes in subject wizard
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/ExamMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15015" windowHeight="6330" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CategorySubjectMappingData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="53">
   <si>
     <t>Academic Year</t>
   </si>
@@ -118,9 +118,6 @@
     <t>New Pre Nursery</t>
   </si>
   <si>
-    <t>New Pre Nursery-1</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -196,8 +193,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -265,7 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,7 +355,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -394,7 +389,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,20 +564,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -597,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -618,21 +612,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -649,7 +643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -673,14 +667,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -688,42 +682,42 @@
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
@@ -735,14 +729,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
@@ -752,42 +746,42 @@
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
@@ -799,48 +793,48 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -853,14 +847,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -868,27 +862,27 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -899,16 +893,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -919,14 +913,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>47</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -935,29 +929,29 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -970,21 +964,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -999,12 +993,12 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -1021,21 +1015,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1069,21 +1063,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1118,21 +1112,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1146,15 +1140,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>29</v>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -1166,21 +1160,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1214,21 +1208,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1242,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1262,21 +1256,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1293,7 +1287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1316,21 +1310,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1347,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1371,14 +1365,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -1386,7 +1380,7 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1403,7 +1397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>